<commit_message>
Cambio de planes, Jesús
</commit_message>
<xml_diff>
--- a/planeacion/Planeacion_Sistema.xlsx
+++ b/planeacion/Planeacion_Sistema.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="35">
   <si>
     <t>Lista de actividades</t>
   </si>
@@ -118,6 +118,9 @@
   </si>
   <si>
     <t>Fecha final:</t>
+  </si>
+  <si>
+    <t>Manual de usuario</t>
   </si>
 </sst>
 </file>
@@ -459,7 +462,7 @@
   <dimension ref="A1:F16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -549,16 +552,16 @@
         <v>4</v>
       </c>
       <c r="B8" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C8" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="D8" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="E8" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
@@ -628,10 +631,18 @@
         <v>32</v>
       </c>
       <c r="B13" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="E13" t="s">
         <v>33</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>34</v>
+      </c>
+      <c r="B14" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Actualización de la planeación del sistema
</commit_message>
<xml_diff>
--- a/planeacion/Planeacion_Sistema.xlsx
+++ b/planeacion/Planeacion_Sistema.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="38">
   <si>
     <t>Lista de actividades</t>
   </si>
@@ -121,6 +121,15 @@
   </si>
   <si>
     <t>Manual de usuario</t>
+  </si>
+  <si>
+    <t>Creación de C.U.</t>
+  </si>
+  <si>
+    <t>Creación de prototipos</t>
+  </si>
+  <si>
+    <t>Integración de CSS a sistema</t>
   </si>
 </sst>
 </file>
@@ -459,10 +468,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F16"/>
+  <dimension ref="A1:F19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -566,10 +575,10 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="B9" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="C9" t="s">
         <v>25</v>
@@ -583,81 +592,132 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>24</v>
+        <v>36</v>
       </c>
       <c r="B10" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="C10" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D10" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E10" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>29</v>
+        <v>37</v>
       </c>
       <c r="B11" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="C11" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D11" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="E11" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>30</v>
+      </c>
+      <c r="B12" t="s">
+        <v>15</v>
+      </c>
       <c r="C12" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="D12" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="E12" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="B13" t="s">
-        <v>21</v>
+        <v>14</v>
+      </c>
+      <c r="C13" t="s">
+        <v>26</v>
+      </c>
+      <c r="D13" t="s">
+        <v>26</v>
       </c>
       <c r="E13" t="s">
-        <v>33</v>
+        <v>18</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="B14" t="s">
-        <v>21</v>
+        <v>20</v>
+      </c>
+      <c r="C14" t="s">
+        <v>27</v>
+      </c>
+      <c r="D14" t="s">
+        <v>27</v>
+      </c>
+      <c r="E14" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>10</v>
-      </c>
-      <c r="B15" t="s">
-        <v>14</v>
+      <c r="C15" t="s">
+        <v>28</v>
+      </c>
+      <c r="D15" t="s">
+        <v>28</v>
+      </c>
+      <c r="E15" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
+        <v>32</v>
+      </c>
+      <c r="B16" t="s">
+        <v>21</v>
+      </c>
+      <c r="E16" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>34</v>
+      </c>
+      <c r="B17" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>10</v>
+      </c>
+      <c r="B18" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
         <v>8</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B19" t="s">
         <v>15</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Especificación del sistema y casos de uso
</commit_message>
<xml_diff>
--- a/planeacion/Planeacion_Sistema.xlsx
+++ b/planeacion/Planeacion_Sistema.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="45">
   <si>
     <t>Lista de actividades</t>
   </si>
@@ -130,6 +130,27 @@
   </si>
   <si>
     <t>Integración de CSS a sistema</t>
+  </si>
+  <si>
+    <t>Casos de uso:</t>
+  </si>
+  <si>
+    <t>iniciar sesión (usuarios)</t>
+  </si>
+  <si>
+    <t>revisión de horarios (administrador)</t>
+  </si>
+  <si>
+    <t>visualizar e imprimir horarios (maestros)</t>
+  </si>
+  <si>
+    <t>altas bajas cambios horario (maestros)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">El maestro inicia sesión indicando usuario, contraseña y carrera, arma su horario y lo guarda en el sistema, el administrador puede ver el horario del maestro y lo acepta o lo rechaza con un comentario explicando el motivo del rechazo del horario y guarda el horario en el sistema, el maestro revisa el horario con comentarios y lo modifica y vuelve a guardarlo en el sistema, el administrador vuelve a revisar el horario y ahora ya lo acepta y lo guarda en sistema, el maestro una vez que su horario fue aceptado ya no puede hacer cambios solo puede visualizarlo e imprimirlo hasta que el administrador del sistema vuelva a habiliar la creación y modificación de horarios, una vez habilitada la opción de actualizar horarios por el administrador, el maestro podrá realizar cambios a su horario definido anteriormente, o eliminarlo y armar uno nuevo, en cada horario va especificado el salón, la experiencia educativa, el número de créditos y el horario de clases. El administrador puede ver los horarios por maestros, por carreras, por salones o por experiencias educativas. El maestro puede configurar sus datos personales en el sistema: nombre del maestro, clave, carrera, experiencia educativa o experiencias educativas. </t>
+  </si>
+  <si>
+    <t>editar datos personales (maestros)</t>
   </si>
 </sst>
 </file>
@@ -165,8 +186,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -468,10 +495,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F19"/>
+  <dimension ref="A1:F26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
+      <selection activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -697,7 +724,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>34</v>
       </c>
@@ -705,7 +732,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>10</v>
       </c>
@@ -713,7 +740,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>8</v>
       </c>
@@ -721,7 +748,49 @@
         <v>15</v>
       </c>
     </row>
+    <row r="20" spans="1:5" s="1" customFormat="1" ht="162" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B20" s="2"/>
+      <c r="C20" s="2"/>
+      <c r="D20" s="2"/>
+      <c r="E20" s="2"/>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>40</v>
+      </c>
+    </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A20:E20"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
Ajustes a la planeación
</commit_message>
<xml_diff>
--- a/planeacion/Planeacion_Sistema.xlsx
+++ b/planeacion/Planeacion_Sistema.xlsx
@@ -497,8 +497,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
-      <selection activeCell="A24" sqref="A24"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="A20" sqref="A20:E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -659,10 +659,10 @@
         <v>15</v>
       </c>
       <c r="C12" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D12" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="E12" t="s">
         <v>18</v>

</xml_diff>

<commit_message>
cambios y casos de uso
</commit_message>
<xml_diff>
--- a/planeacion/Planeacion_Sistema.xlsx
+++ b/planeacion/Planeacion_Sistema.xlsx
@@ -189,7 +189,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -197,11 +197,26 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -209,6 +224,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -513,7 +529,7 @@
   <dimension ref="A1:G27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+      <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -521,8 +537,8 @@
     <col min="1" max="1" width="46.28515625" customWidth="1"/>
     <col min="2" max="2" width="13.140625" customWidth="1"/>
     <col min="3" max="3" width="22.28515625" customWidth="1"/>
-    <col min="4" max="4" width="17" customWidth="1"/>
-    <col min="5" max="5" width="16.7109375" customWidth="1"/>
+    <col min="4" max="4" width="33.7109375" customWidth="1"/>
+    <col min="5" max="5" width="27.7109375" customWidth="1"/>
     <col min="6" max="6" width="11.140625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -759,36 +775,36 @@
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
+      <c r="A16" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B16" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="C16" t="s">
+      <c r="C16" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="D16" t="s">
+      <c r="D16" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="E16" t="s">
+      <c r="E16" s="3" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
+      <c r="A17" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B17" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="C17" t="s">
+      <c r="C17" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="D17" t="s">
+      <c r="D17" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="E17" t="s">
+      <c r="E17" s="3" t="s">
         <v>16</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Actualizacion de la documentacion
</commit_message>
<xml_diff>
--- a/planeacion/Planeacion_Sistema.xlsx
+++ b/planeacion/Planeacion_Sistema.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="55">
   <si>
     <t>Lista de actividades</t>
   </si>
@@ -178,13 +178,16 @@
   </si>
   <si>
     <t>Elaboración de: Modelo E-R, Especificación de los C.U., elaboración del diccionario de datos, integración con el manual de usuario</t>
+  </si>
+  <si>
+    <t>Horas de trabajo</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -192,16 +195,34 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -224,11 +245,48 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -236,7 +294,41 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -538,10 +630,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G31"/>
+  <dimension ref="A1:I31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A21" sqref="A21"/>
+      <selection sqref="A1:I24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -550,327 +642,458 @@
     <col min="2" max="2" width="13.140625" customWidth="1"/>
     <col min="3" max="3" width="22.28515625" customWidth="1"/>
     <col min="4" max="4" width="17" customWidth="1"/>
-    <col min="5" max="5" width="16.7109375" customWidth="1"/>
+    <col min="5" max="5" width="17.42578125" customWidth="1"/>
     <col min="6" max="6" width="11.140625" customWidth="1"/>
+    <col min="7" max="7" width="18.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="3" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="G1" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="H1" s="5"/>
+      <c r="I1" s="6"/>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="7" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="C2" s="7"/>
+      <c r="D2" s="7"/>
+      <c r="E2" s="7"/>
+      <c r="F2" s="7"/>
+      <c r="G2" s="8"/>
+      <c r="H2" s="9"/>
+      <c r="I2" s="10"/>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" s="7" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="B3" s="7"/>
+      <c r="C3" s="7"/>
+      <c r="D3" s="7"/>
+      <c r="E3" s="7"/>
+      <c r="F3" s="7"/>
+      <c r="G3" s="8"/>
+      <c r="H3" s="9"/>
+      <c r="I3" s="10"/>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" s="7"/>
+      <c r="B4" s="7"/>
+      <c r="C4" s="7"/>
+      <c r="D4" s="7"/>
+      <c r="E4" s="7"/>
+      <c r="F4" s="11"/>
+      <c r="G4" s="8"/>
+      <c r="H4" s="9"/>
+      <c r="I4" s="10"/>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" s="7" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+      <c r="B5" s="7"/>
+      <c r="C5" s="7"/>
+      <c r="D5" s="7"/>
+      <c r="E5" s="7"/>
+      <c r="F5" s="11"/>
+      <c r="G5" s="8"/>
+      <c r="H5" s="9"/>
+      <c r="I5" s="10"/>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D6" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="E6" t="s">
+      <c r="E6" s="7" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+      <c r="F6" s="7"/>
+      <c r="G6" s="8"/>
+      <c r="H6" s="9"/>
+      <c r="I6" s="10"/>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D7" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="E7" t="s">
+      <c r="E7" s="7" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+      <c r="F7" s="7"/>
+      <c r="G7" s="8"/>
+      <c r="H7" s="9"/>
+      <c r="I7" s="10"/>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C8" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="D8" t="s">
+      <c r="D8" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="E8" t="s">
+      <c r="E8" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="F8">
+      <c r="F8" s="7">
         <v>80</v>
       </c>
-      <c r="G8" t="s">
+      <c r="G8" s="8" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+      <c r="H8" s="9"/>
+      <c r="I8" s="10"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C9" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="D9" t="s">
+      <c r="D9" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="E9" t="s">
+      <c r="E9" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="F9">
+      <c r="F9" s="7">
         <v>60</v>
       </c>
-      <c r="G9" t="s">
+      <c r="G9" s="8" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+      <c r="H9" s="9"/>
+      <c r="I9" s="10"/>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C10" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="D10" t="s">
+      <c r="D10" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="E10" t="s">
+      <c r="E10" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="F10">
+      <c r="F10" s="7">
         <v>75</v>
       </c>
-      <c r="G10" t="s">
+      <c r="G10" s="8" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+      <c r="H10" s="9"/>
+      <c r="I10" s="10"/>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C11" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="D11" t="s">
+      <c r="D11" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="E11" t="s">
+      <c r="E11" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="F11">
+      <c r="F11" s="7">
         <v>90</v>
       </c>
-      <c r="G11" t="s">
+      <c r="G11" s="8" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+      <c r="H11" s="9"/>
+      <c r="I11" s="10"/>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B12" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C12" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="D12" t="s">
+      <c r="D12" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="E12" t="s">
+      <c r="E12" s="7" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+      <c r="F12" s="7"/>
+      <c r="G12" s="8"/>
+      <c r="H12" s="9"/>
+      <c r="I12" s="10"/>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" s="8" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
+      <c r="B13" s="9"/>
+      <c r="C13" s="9"/>
+      <c r="D13" s="9"/>
+      <c r="E13" s="9"/>
+      <c r="F13" s="10"/>
+      <c r="G13" s="8"/>
+      <c r="H13" s="9"/>
+      <c r="I13" s="10"/>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B14" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="C14" t="s">
+      <c r="C14" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="D14" t="s">
+      <c r="D14" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="E14" t="s">
+      <c r="E14" s="7" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
+      <c r="F14" s="7"/>
+      <c r="G14" s="8"/>
+      <c r="H14" s="9"/>
+      <c r="I14" s="10"/>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15" s="7" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
+      <c r="B15" s="7"/>
+      <c r="C15" s="7"/>
+      <c r="D15" s="7"/>
+      <c r="E15" s="7"/>
+      <c r="F15" s="7"/>
+      <c r="G15" s="8"/>
+      <c r="H15" s="9"/>
+      <c r="I15" s="10"/>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B16" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="C16" t="s">
+      <c r="C16" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="D16" t="s">
+      <c r="D16" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="E16" t="s">
+      <c r="E16" s="7" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
+      <c r="F16" s="7"/>
+      <c r="G16" s="8"/>
+      <c r="H16" s="9"/>
+      <c r="I16" s="10"/>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A17" s="8" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="3" t="s">
+      <c r="B17" s="9"/>
+      <c r="C17" s="9"/>
+      <c r="D17" s="9"/>
+      <c r="E17" s="9"/>
+      <c r="F17" s="9"/>
+      <c r="G17" s="9"/>
+      <c r="H17" s="9"/>
+      <c r="I17" s="10"/>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A18" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="B18" s="3" t="s">
+      <c r="B18" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="C18" s="3" t="s">
+      <c r="C18" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="D18" s="3" t="s">
+      <c r="D18" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="E18" s="3" t="s">
+      <c r="E18" s="7" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
+      <c r="F18" s="7"/>
+      <c r="G18" s="8"/>
+      <c r="H18" s="9"/>
+      <c r="I18" s="10"/>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A19" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B19" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="C19" t="s">
+      <c r="C19" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="D19" t="s">
+      <c r="D19" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="E19" t="s">
+      <c r="E19" s="7" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
+      <c r="F19" s="7"/>
+      <c r="G19" s="8"/>
+      <c r="H19" s="9"/>
+      <c r="I19" s="10"/>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A20" s="7" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
+      <c r="B20" s="7"/>
+      <c r="C20" s="7"/>
+      <c r="D20" s="7"/>
+      <c r="E20" s="7"/>
+      <c r="F20" s="7"/>
+      <c r="G20" s="8"/>
+      <c r="H20" s="9"/>
+      <c r="I20" s="10"/>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A21" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B21" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="C21" t="s">
+      <c r="C21" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="D21" t="s">
+      <c r="D21" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="E21" t="s">
+      <c r="E21" s="7" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
+      <c r="F21" s="7"/>
+      <c r="G21" s="8"/>
+      <c r="H21" s="9"/>
+      <c r="I21" s="10"/>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A22" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="B22" t="s">
+      <c r="B22" s="7" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
+      <c r="C22" s="7"/>
+      <c r="D22" s="7"/>
+      <c r="E22" s="7"/>
+      <c r="F22" s="7"/>
+      <c r="G22" s="8"/>
+      <c r="H22" s="9"/>
+      <c r="I22" s="10"/>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A23" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="B23" t="s">
+      <c r="B23" s="7" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="24" spans="1:5" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B24" t="s">
+      <c r="C23" s="7"/>
+      <c r="D23" s="7"/>
+      <c r="E23" s="7"/>
+      <c r="F23" s="7"/>
+      <c r="G23" s="8"/>
+      <c r="H23" s="9"/>
+      <c r="I23" s="10"/>
+    </row>
+    <row r="24" spans="1:9" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="12"/>
+      <c r="B24" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="C24" t="s">
+      <c r="C24" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="D24" t="s">
+      <c r="D24" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="E24" t="s">
+      <c r="E24" s="7" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="25" spans="1:5" ht="166.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F24" s="12"/>
+      <c r="G24" s="13"/>
+      <c r="H24" s="14"/>
+      <c r="I24" s="15"/>
+    </row>
+    <row r="25" spans="1:9" ht="166.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
         <v>43</v>
       </c>
@@ -879,41 +1102,67 @@
       <c r="D25" s="2"/>
       <c r="E25" s="2"/>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>40</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="26">
+    <mergeCell ref="G24:I24"/>
+    <mergeCell ref="G19:I19"/>
+    <mergeCell ref="G20:I20"/>
+    <mergeCell ref="G21:I21"/>
+    <mergeCell ref="G22:I22"/>
+    <mergeCell ref="G23:I23"/>
+    <mergeCell ref="G13:I13"/>
+    <mergeCell ref="G14:I14"/>
+    <mergeCell ref="G15:I15"/>
+    <mergeCell ref="G16:I16"/>
+    <mergeCell ref="G18:I18"/>
     <mergeCell ref="A25:E25"/>
+    <mergeCell ref="A17:I17"/>
+    <mergeCell ref="G1:I1"/>
+    <mergeCell ref="G2:I2"/>
+    <mergeCell ref="G3:I3"/>
+    <mergeCell ref="G4:I4"/>
+    <mergeCell ref="G5:I5"/>
+    <mergeCell ref="G6:I6"/>
+    <mergeCell ref="G7:I7"/>
+    <mergeCell ref="G8:I8"/>
+    <mergeCell ref="G9:I9"/>
+    <mergeCell ref="G10:I10"/>
+    <mergeCell ref="G11:I11"/>
+    <mergeCell ref="A13:F13"/>
+    <mergeCell ref="G12:I12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>